<commit_message>
analyse sur les graphes
</commit_message>
<xml_diff>
--- a/N_Reines.xlsx
+++ b/N_Reines.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B755FA43-811F-4F8B-8661-74AD48A13EFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C15796-7802-4A1A-875A-BB2D6B3756B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="data_queens" sheetId="1" r:id="rId1"/>
+    <sheet name="analysis_queens" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -108,7 +108,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -212,7 +212,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -374,7 +374,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$53</c:f>
+              <c:f>data_queens!$D$3:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -555,7 +555,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -717,7 +717,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$53</c:f>
+              <c:f>data_queens!$L$3:$L$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -898,7 +898,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1060,7 +1060,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$3:$T$53</c:f>
+              <c:f>data_queens!$T$3:$T$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1253,7 +1253,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1415,7 +1415,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AB$3:$AB$53</c:f>
+              <c:f>data_queens!$AB$3:$AB$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1910,7 +1910,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2014,7 +2014,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2176,7 +2176,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$53</c:f>
+              <c:f>data_queens!$B$3:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2375,7 +2375,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2537,7 +2537,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$53</c:f>
+              <c:f>data_queens!$J$3:$J$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2736,7 +2736,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2898,7 +2898,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$3:$R$53</c:f>
+              <c:f>data_queens!$R$3:$R$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3097,7 +3097,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3259,7 +3259,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$3:$Z$53</c:f>
+              <c:f>data_queens!$Z$3:$Z$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3761,7 +3761,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3865,7 +3865,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -4027,7 +4027,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$53</c:f>
+              <c:f>data_queens!$D$3:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -4208,7 +4208,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -4370,7 +4370,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$53</c:f>
+              <c:f>data_queens!$L$3:$L$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -4551,7 +4551,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -4713,7 +4713,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$3:$T$53</c:f>
+              <c:f>data_queens!$T$3:$T$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -4906,7 +4906,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$53</c:f>
+              <c:f>data_queens!$A$3:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -5068,7 +5068,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AB$3:$AB$53</c:f>
+              <c:f>data_queens!$AB$3:$AB$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -7615,11 +7615,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -11961,11 +11961,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFA2DEB-E6E3-4635-BE5A-4409763A9C19}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>